<commit_message>
Update packages & docs
</commit_message>
<xml_diff>
--- a/samples/openai-acs-msgraph/customer documents/Adventure-Works-Cycles-Supplies.xlsx
+++ b/samples/openai-acs-msgraph/customer documents/Adventure-Works-Cycles-Supplies.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danwahlin/Desktop/projects/openai-acs-msgraph/customer documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375C52AA-499F-1247-96E5-06F90225D8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43160" yWindow="500" windowWidth="30200" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +32,196 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+  <si>
+    <t>productId</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>shippedDate</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Mountain Bike</t>
+  </si>
+  <si>
+    <t>Bikes</t>
+  </si>
+  <si>
+    <t>Road Bike</t>
+  </si>
+  <si>
+    <t>Hybrid Bike</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Bike Lock</t>
+  </si>
+  <si>
+    <t>Bike Pump</t>
+  </si>
+  <si>
+    <t>Cycling Shorts</t>
+  </si>
+  <si>
+    <t>Apparel</t>
+  </si>
+  <si>
+    <t>Cycling Jersey</t>
+  </si>
+  <si>
+    <t>Cycling Shoes</t>
+  </si>
+  <si>
+    <t>Cycling Gloves</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>customerEmail</t>
+  </si>
+  <si>
+    <t>shippingAddress</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>johnsmith@example.com</t>
+  </si>
+  <si>
+    <t>123 Main St, Anytown, USA</t>
+  </si>
+  <si>
+    <t>Sarah Johnson</t>
+  </si>
+  <si>
+    <t>sarahjohnson@example.com</t>
+  </si>
+  <si>
+    <t>456 Elm St, Anycity, USA</t>
+  </si>
+  <si>
+    <t>Michael Brown</t>
+  </si>
+  <si>
+    <t>mbrown@example.com</t>
+  </si>
+  <si>
+    <t>789 Oak Ave, Anyville, USA</t>
+  </si>
+  <si>
+    <t>Emily Davis</t>
+  </si>
+  <si>
+    <t>emilydavis@example.com</t>
+  </si>
+  <si>
+    <t>321 Maple Rd, Anyborough, USA</t>
+  </si>
+  <si>
+    <t>David Wilson</t>
+  </si>
+  <si>
+    <t>dwilson@example.com</t>
+  </si>
+  <si>
+    <t>654 Pine Ln, Anyvillage, USA</t>
+  </si>
+  <si>
+    <t>Olivia Taylor</t>
+  </si>
+  <si>
+    <t>otaylor@example.com</t>
+  </si>
+  <si>
+    <t>987 Cedar St, Anyhamlet, USA</t>
+  </si>
+  <si>
+    <t>James Anderson</t>
+  </si>
+  <si>
+    <t>janderson@example.com</t>
+  </si>
+  <si>
+    <t>567 Birch Ave, Anytown, USA</t>
+  </si>
+  <si>
+    <t>Emma Thompson</t>
+  </si>
+  <si>
+    <t>ethompson@example.com</t>
+  </si>
+  <si>
+    <t>876 Oak St, Anycity, USA</t>
+  </si>
+  <si>
+    <t>Daniel Martinez</t>
+  </si>
+  <si>
+    <t>dmartinez@example.com</t>
+  </si>
+  <si>
+    <t>345 Elm Rd, Anyville, USA</t>
+  </si>
+  <si>
+    <t>Sophia Garcia</t>
+  </si>
+  <si>
+    <t>sgarcia@example.com</t>
+  </si>
+  <si>
+    <t>654 Pine Ln, Anyborough, USA</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="#,##0.00;[Red]#,##0.00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,13 +244,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,12 +574,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45078</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1599.99</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45079</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1999.99</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45079</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8">
+        <v>899.99</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45080</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45081</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45082</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8">
+        <v>29.99</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45083</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8">
+        <v>49.99</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45084</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8">
+        <v>59.99</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45085</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8">
+        <v>99.99</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45086</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="mailto:johnsmith@example.com" xr:uid="{9F2198E2-C47D-914C-BE20-53C53A078397}"/>
+    <hyperlink ref="H3" r:id="rId2" display="mailto:sarahjohnson@example.com" xr:uid="{255E6CAD-D808-A447-B606-4452D9086B3C}"/>
+    <hyperlink ref="H4" r:id="rId3" display="mailto:mbrown@example.com" xr:uid="{50A050FC-539F-D644-9BD6-58A69AF175A8}"/>
+    <hyperlink ref="H5" r:id="rId4" display="mailto:emilydavis@example.com" xr:uid="{4E7C18DD-6E2F-2246-8489-306D3DBEDAC3}"/>
+    <hyperlink ref="H6" r:id="rId5" display="mailto:dwilson@example.com" xr:uid="{F9624D38-ADBC-2B48-9AEF-91FBAC284D9D}"/>
+    <hyperlink ref="H7" r:id="rId6" display="mailto:otaylor@example.com" xr:uid="{640E8E29-2594-684E-B4AE-C61EAA0FC559}"/>
+    <hyperlink ref="H8" r:id="rId7" display="mailto:janderson@example.com" xr:uid="{539706D7-08D6-EE47-924C-210E03D567BD}"/>
+    <hyperlink ref="H9" r:id="rId8" display="mailto:ethompson@example.com" xr:uid="{6087C50C-4312-D14E-AEAA-E1005F69C957}"/>
+    <hyperlink ref="H10" r:id="rId9" display="mailto:dmartinez@example.com" xr:uid="{8074D944-1D98-A54E-8EBA-C9CD1D763B41}"/>
+    <hyperlink ref="H11" r:id="rId10" display="mailto:sgarcia@example.com" xr:uid="{A0216223-8A75-8F46-A15C-077199A66849}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>